<commit_message>
Added yearly justified total
</commit_message>
<xml_diff>
--- a/resources/project-breakdown.xlsx
+++ b/resources/project-breakdown.xlsx
@@ -8,33 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmasnada\git\opensource\HourDistributor\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE2681C-7D33-4C31-9ADF-39796136EA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D5B7A0-37F1-4E05-86AB-2E6E555EB901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
-    <sheet name="John Smith" sheetId="1" r:id="rId2"/>
-    <sheet name="report_template" sheetId="2" r:id="rId3"/>
-    <sheet name="John Smith - 2023" sheetId="5" r:id="rId4"/>
+    <sheet name="report_template" sheetId="2" r:id="rId2"/>
+    <sheet name="John Smith" sheetId="1" r:id="rId3"/>
+    <sheet name="John Smith - 2023" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="all_prj_justified" localSheetId="3">'John Smith - 2023'!$C$7:$C$30</definedName>
-    <definedName name="all_prj_justified_total" localSheetId="3">'John Smith - 2023'!$C$32</definedName>
-    <definedName name="all_prj_monthly_justified_1" localSheetId="3">'John Smith - 2023'!$D$7:$D$30</definedName>
-    <definedName name="all_prj_monthly_justified_10" localSheetId="3">'John Smith - 2023'!$M$7:$M$30</definedName>
-    <definedName name="all_prj_monthly_justified_11" localSheetId="3">'John Smith - 2023'!$N$7:$N$30</definedName>
-    <definedName name="all_prj_monthly_justified_12" localSheetId="3">'John Smith - 2023'!$O$7:$O$30</definedName>
-    <definedName name="all_prj_monthly_justified_2" localSheetId="3">'John Smith - 2023'!$E$7:$E$30</definedName>
-    <definedName name="all_prj_monthly_justified_3" localSheetId="3">'John Smith - 2023'!$F$7:$F$30</definedName>
-    <definedName name="all_prj_monthly_justified_4" localSheetId="3">'John Smith - 2023'!$G$7:$G$30</definedName>
-    <definedName name="all_prj_monthly_justified_5" localSheetId="3">'John Smith - 2023'!$H$7:$H$30</definedName>
-    <definedName name="all_prj_monthly_justified_6" localSheetId="3">'John Smith - 2023'!$I$7:$I$30</definedName>
-    <definedName name="all_prj_monthly_justified_7" localSheetId="3">'John Smith - 2023'!$J$7:$J$30</definedName>
-    <definedName name="all_prj_monthly_justified_8" localSheetId="3">'John Smith - 2023'!$K$7:$K$30</definedName>
-    <definedName name="all_prj_monthly_justified_9" localSheetId="3">'John Smith - 2023'!$L$7:$L$30</definedName>
-    <definedName name="all_prj_projected" localSheetId="3">'John Smith - 2023'!$B$7:$B$30</definedName>
-    <definedName name="all_prj_projected_total" localSheetId="3">'John Smith - 2023'!$B$32</definedName>
+    <definedName name="all_prj_justified" localSheetId="3">'John Smith - 2023'!$C$7:$C$20</definedName>
+    <definedName name="all_prj_justified_total" localSheetId="3">'John Smith - 2023'!$C$22</definedName>
+    <definedName name="all_prj_monthly_justified_1" localSheetId="3">'John Smith - 2023'!$D$7:$D$20</definedName>
+    <definedName name="all_prj_monthly_justified_10" localSheetId="3">'John Smith - 2023'!$M$7:$M$20</definedName>
+    <definedName name="all_prj_monthly_justified_11" localSheetId="3">'John Smith - 2023'!$N$7:$N$20</definedName>
+    <definedName name="all_prj_monthly_justified_12" localSheetId="3">'John Smith - 2023'!$O$7:$O$20</definedName>
+    <definedName name="all_prj_monthly_justified_2" localSheetId="3">'John Smith - 2023'!$E$7:$E$20</definedName>
+    <definedName name="all_prj_monthly_justified_3" localSheetId="3">'John Smith - 2023'!$F$7:$F$20</definedName>
+    <definedName name="all_prj_monthly_justified_4" localSheetId="3">'John Smith - 2023'!$G$7:$G$20</definedName>
+    <definedName name="all_prj_monthly_justified_5" localSheetId="3">'John Smith - 2023'!$H$7:$H$20</definedName>
+    <definedName name="all_prj_monthly_justified_6" localSheetId="3">'John Smith - 2023'!$I$7:$I$20</definedName>
+    <definedName name="all_prj_monthly_justified_7" localSheetId="3">'John Smith - 2023'!$J$7:$J$20</definedName>
+    <definedName name="all_prj_monthly_justified_8" localSheetId="3">'John Smith - 2023'!$K$7:$K$20</definedName>
+    <definedName name="all_prj_monthly_justified_9" localSheetId="3">'John Smith - 2023'!$L$7:$L$20</definedName>
+    <definedName name="all_prj_projected" localSheetId="3">'John Smith - 2023'!$B$7:$B$20</definedName>
+    <definedName name="all_prj_projected_total" localSheetId="3">'John Smith - 2023'!$B$22</definedName>
     <definedName name="employee" localSheetId="3">'John Smith - 2023'!$B$2</definedName>
     <definedName name="justification_year" localSheetId="3">'John Smith - 2023'!$B$3</definedName>
     <definedName name="max_yearly_limit" localSheetId="3">'John Smith - 2023'!$B$4</definedName>
@@ -51,17 +51,17 @@
     <definedName name="prj_monthly_justified_pertevec_at9" localSheetId="3">'John Smith - 2023'!$D$17:$O$17</definedName>
     <definedName name="prj_monthly_justified_pilas" localSheetId="3">'John Smith - 2023'!$D$18:$O$18</definedName>
     <definedName name="prj_monthly_justified_porcino" localSheetId="3">'John Smith - 2023'!$D$19:$O$19</definedName>
-    <definedName name="prj_monthly_justified_redol_wp1" localSheetId="3">'John Smith - 2023'!$D$20:$O$20</definedName>
-    <definedName name="prj_monthly_justified_redol_wp2" localSheetId="3">'John Smith - 2023'!$D$21:$O$21</definedName>
-    <definedName name="prj_monthly_justified_redol_wp4" localSheetId="3">'John Smith - 2023'!$D$22:$O$22</definedName>
-    <definedName name="prj_monthly_justified_redol_wp7" localSheetId="3">'John Smith - 2023'!$D$23:$O$23</definedName>
-    <definedName name="prj_monthly_justified_redol_wp8" localSheetId="3">'John Smith - 2023'!$D$24:$O$24</definedName>
-    <definedName name="prj_monthly_justified_reset" localSheetId="3">'John Smith - 2023'!$D$25:$O$25</definedName>
-    <definedName name="prj_monthly_justified_treasure_wp4" localSheetId="3">'John Smith - 2023'!$D$26:$O$26</definedName>
-    <definedName name="prj_monthly_justified_treasure_wp6" localSheetId="3">'John Smith - 2023'!$D$27:$O$27</definedName>
-    <definedName name="prj_monthly_justified_treasure_wp7" localSheetId="3">'John Smith - 2023'!$D$28:$O$28</definedName>
-    <definedName name="prj_monthly_justified_treasure_wp8" localSheetId="3">'John Smith - 2023'!$D$29:$O$29</definedName>
-    <definedName name="prj_monthly_justified_treasure_wp9" localSheetId="3">'John Smith - 2023'!$D$30:$O$30</definedName>
+    <definedName name="prj_monthly_justified_redol_wp1" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_monthly_justified_redol_wp2" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_monthly_justified_redol_wp4" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_monthly_justified_redol_wp7" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_monthly_justified_redol_wp8" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_monthly_justified_reset" localSheetId="3">'John Smith - 2023'!$D$20:$O$20</definedName>
+    <definedName name="prj_monthly_justified_treasure_wp4" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_monthly_justified_treasure_wp6" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_monthly_justified_treasure_wp7" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_monthly_justified_treasure_wp8" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_monthly_justified_treasure_wp9" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
     <definedName name="prj_total_justified_bioestilas" localSheetId="3">'John Smith - 2023'!$C$7</definedName>
     <definedName name="prj_total_justified_ensure" localSheetId="3">'John Smith - 2023'!$C$8</definedName>
     <definedName name="prj_total_justified_h2pcomplementario" localSheetId="3">'John Smith - 2023'!$C$9</definedName>
@@ -75,17 +75,17 @@
     <definedName name="prj_total_justified_pertevec_at9" localSheetId="3">'John Smith - 2023'!$C$17</definedName>
     <definedName name="prj_total_justified_pilas" localSheetId="3">'John Smith - 2023'!$C$18</definedName>
     <definedName name="prj_total_justified_porcino" localSheetId="3">'John Smith - 2023'!$C$19</definedName>
-    <definedName name="prj_total_justified_redol_wp1" localSheetId="3">'John Smith - 2023'!$C$20</definedName>
-    <definedName name="prj_total_justified_redol_wp2" localSheetId="3">'John Smith - 2023'!$C$21</definedName>
-    <definedName name="prj_total_justified_redol_wp4" localSheetId="3">'John Smith - 2023'!$C$22</definedName>
-    <definedName name="prj_total_justified_redol_wp7" localSheetId="3">'John Smith - 2023'!$C$23</definedName>
-    <definedName name="prj_total_justified_redol_wp8" localSheetId="3">'John Smith - 2023'!$C$24</definedName>
-    <definedName name="prj_total_justified_reset" localSheetId="3">'John Smith - 2023'!$C$25</definedName>
-    <definedName name="prj_total_justified_treasure_wp4" localSheetId="3">'John Smith - 2023'!$C$26</definedName>
-    <definedName name="prj_total_justified_treasure_wp6" localSheetId="3">'John Smith - 2023'!$C$27</definedName>
-    <definedName name="prj_total_justified_treasure_wp7" localSheetId="3">'John Smith - 2023'!$C$28</definedName>
-    <definedName name="prj_total_justified_treasure_wp8" localSheetId="3">'John Smith - 2023'!$C$29</definedName>
-    <definedName name="prj_total_justified_treasure_wp9" localSheetId="3">'John Smith - 2023'!$C$30</definedName>
+    <definedName name="prj_total_justified_redol_wp1" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_justified_redol_wp2" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_justified_redol_wp4" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_justified_redol_wp7" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_justified_redol_wp8" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_justified_reset" localSheetId="3">'John Smith - 2023'!$C$20</definedName>
+    <definedName name="prj_total_justified_treasure_wp4" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_justified_treasure_wp6" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_justified_treasure_wp7" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_justified_treasure_wp8" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_justified_treasure_wp9" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
     <definedName name="prj_total_projected_bioestilas" localSheetId="3">'John Smith - 2023'!$B$7</definedName>
     <definedName name="prj_total_projected_ensure" localSheetId="3">'John Smith - 2023'!$B$8</definedName>
     <definedName name="prj_total_projected_h2pcomplementario" localSheetId="3">'John Smith - 2023'!$B$9</definedName>
@@ -99,17 +99,17 @@
     <definedName name="prj_total_projected_pertevec_at9" localSheetId="3">'John Smith - 2023'!$B$17</definedName>
     <definedName name="prj_total_projected_pilas" localSheetId="3">'John Smith - 2023'!$B$18</definedName>
     <definedName name="prj_total_projected_porcino" localSheetId="3">'John Smith - 2023'!$B$19</definedName>
-    <definedName name="prj_total_projected_redol_wp1" localSheetId="3">'John Smith - 2023'!$B$20</definedName>
-    <definedName name="prj_total_projected_redol_wp2" localSheetId="3">'John Smith - 2023'!$B$21</definedName>
-    <definedName name="prj_total_projected_redol_wp4" localSheetId="3">'John Smith - 2023'!$B$22</definedName>
-    <definedName name="prj_total_projected_redol_wp7" localSheetId="3">'John Smith - 2023'!$B$23</definedName>
-    <definedName name="prj_total_projected_redol_wp8" localSheetId="3">'John Smith - 2023'!$B$24</definedName>
-    <definedName name="prj_total_projected_reset" localSheetId="3">'John Smith - 2023'!$B$25</definedName>
-    <definedName name="prj_total_projected_treasure_wp4" localSheetId="3">'John Smith - 2023'!$B$26</definedName>
-    <definedName name="prj_total_projected_treasure_wp6" localSheetId="3">'John Smith - 2023'!$B$27</definedName>
-    <definedName name="prj_total_projected_treasure_wp7" localSheetId="3">'John Smith - 2023'!$B$28</definedName>
-    <definedName name="prj_total_projected_treasure_wp8" localSheetId="3">'John Smith - 2023'!$B$29</definedName>
-    <definedName name="prj_total_projected_treasure_wp9" localSheetId="3">'John Smith - 2023'!$B$30</definedName>
+    <definedName name="prj_total_projected_redol_wp1" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_projected_redol_wp2" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_projected_redol_wp4" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_projected_redol_wp7" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_projected_redol_wp8" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_projected_reset" localSheetId="3">'John Smith - 2023'!$B$20</definedName>
+    <definedName name="prj_total_projected_treasure_wp4" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_projected_treasure_wp6" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_projected_treasure_wp7" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_projected_treasure_wp8" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
+    <definedName name="prj_total_projected_treasure_wp9" localSheetId="3">'John Smith - 2023'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -1083,7 +1083,7 @@
     <author>Masnada, Julien Florian Jacques</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{FBA268A4-BBF1-45C9-8550-01336954D55D}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{005F7C9A-D32A-4C8C-8BB5-C7D198FA3CD6}">
       <text>
         <r>
           <rPr>
@@ -1098,7 +1098,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{6A179520-0C84-46A4-AEE1-EB1591D8C7FA}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{1733DB2B-68BC-47E1-B2CB-096C87D97DD1}">
       <text>
         <r>
           <rPr>
@@ -1113,7 +1113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{2F54A694-0657-41EA-B31B-A08843E76DFB}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{E9727C75-621A-4645-BDB7-F5D6781EB8D4}">
       <text>
         <r>
           <rPr>
@@ -1128,7 +1128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{FBD3BB99-A61B-474B-95FA-049518F558B7}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{D751C0A9-CCD2-4D3F-89B6-55B1B3FB69DA}">
       <text>
         <r>
           <rPr>
@@ -1143,7 +1143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{C9E1C6C0-E8BC-46E2-BA06-D58C66D5660A}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{48BC598E-FB6F-4DC9-8825-B697C2017612}">
       <text>
         <r>
           <rPr>
@@ -1158,7 +1158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{E4B6AF5C-45DB-456F-8D78-22F2EE39E87E}">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{9F8032E8-473E-4988-AC2A-CACC0B46B1AA}">
       <text>
         <r>
           <rPr>
@@ -1173,7 +1173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{06D4D586-3FDF-4E42-A32C-FD72D75B26BC}">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{4747D333-2DDE-48D4-B7E4-54675B6AFB85}">
       <text>
         <r>
           <rPr>
@@ -1188,7 +1188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B32" authorId="0" shapeId="0" xr:uid="{D31F69D3-A4C0-447D-BA66-16F262531534}">
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{5F67221F-7A61-412B-AE18-802B416F8A16}">
       <text>
         <r>
           <rPr>
@@ -1203,7 +1203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C32" authorId="0" shapeId="0" xr:uid="{D416A528-E368-4781-875E-1710B6CA25B9}">
+    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{BB936A41-1905-45E9-9BA0-1025860AC2C4}">
       <text>
         <r>
           <rPr>
@@ -1218,7 +1218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D32" authorId="0" shapeId="0" xr:uid="{FD6709A7-73CD-4180-BCD7-A2588C20E65E}">
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{446EC147-FED1-47A6-8E8E-284CE7543A46}">
       <text>
         <r>
           <rPr>
@@ -1234,7 +1234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E32" authorId="0" shapeId="0" xr:uid="{5AA9B077-84D1-4603-856D-32FE7620C428}">
+    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{CE82E5FF-7183-4C31-9BFB-C2FE5E354086}">
       <text>
         <r>
           <rPr>
@@ -1250,7 +1250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{241B1E06-A2F6-446C-8794-F20030D844DF}">
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{81100B88-B6A2-40EE-B575-ADE2F426DD0F}">
       <text>
         <r>
           <rPr>
@@ -1266,7 +1266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G32" authorId="0" shapeId="0" xr:uid="{17E6CA52-F73C-4BB9-9E69-D639619ED430}">
+    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{D36BDE9D-4D40-4E93-B54A-482EEB4D25F5}">
       <text>
         <r>
           <rPr>
@@ -1282,7 +1282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H32" authorId="0" shapeId="0" xr:uid="{C4B8C329-AF63-48A6-B5BE-3F1060B356C1}">
+    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{ACB20B9C-8780-4FFF-AFD7-BC61017AEAD0}">
       <text>
         <r>
           <rPr>
@@ -1298,7 +1298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I32" authorId="0" shapeId="0" xr:uid="{BAE5D9E6-B359-4673-8415-E486EFCA2C1C}">
+    <comment ref="I22" authorId="0" shapeId="0" xr:uid="{BA37C098-1DF5-4242-AD74-6078151B9E7D}">
       <text>
         <r>
           <rPr>
@@ -1314,7 +1314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J32" authorId="0" shapeId="0" xr:uid="{D43FE0A1-8A9C-42B2-B19E-D2219D9563E5}">
+    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{1CC2203E-1DEA-46DF-BE8E-4CEF4B42B0C3}">
       <text>
         <r>
           <rPr>
@@ -1330,7 +1330,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K32" authorId="0" shapeId="0" xr:uid="{0824CCE3-3703-425D-B849-EF5C172B6BF6}">
+    <comment ref="K22" authorId="0" shapeId="0" xr:uid="{62D5BD41-B47D-48A7-8D88-0AD66FA9F924}">
       <text>
         <r>
           <rPr>
@@ -1346,7 +1346,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L32" authorId="0" shapeId="0" xr:uid="{DF0F05ED-ECD5-4EFB-8B86-D44DB18B0D81}">
+    <comment ref="L22" authorId="0" shapeId="0" xr:uid="{F88253D9-3BC8-47AD-9284-8818AB79D2F3}">
       <text>
         <r>
           <rPr>
@@ -1362,7 +1362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M32" authorId="0" shapeId="0" xr:uid="{DCDD61B8-D5E3-44AB-BD69-4B5F03CE5CDC}">
+    <comment ref="M22" authorId="0" shapeId="0" xr:uid="{07528654-D48A-4179-9250-49BBE5BA626D}">
       <text>
         <r>
           <rPr>
@@ -1378,7 +1378,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N32" authorId="0" shapeId="0" xr:uid="{66008816-4F43-4598-99A5-4634BC217B49}">
+    <comment ref="N22" authorId="0" shapeId="0" xr:uid="{2E6EF74C-AE89-4A05-BE70-6416EA0C3B35}">
       <text>
         <r>
           <rPr>
@@ -1394,7 +1394,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O32" authorId="0" shapeId="0" xr:uid="{23B95372-EC26-401D-9C07-8E0B26D70DC0}">
+    <comment ref="O22" authorId="0" shapeId="0" xr:uid="{D0795573-2FC7-4F5A-A2BE-EA024AE7A16A}">
       <text>
         <r>
           <rPr>
@@ -1410,7 +1410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A33" authorId="0" shapeId="0" xr:uid="{B6BAF688-ADEA-4DA0-85ED-69E606478821}">
+    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{90C8857F-6054-43F8-A4CA-24735AB19842}">
       <text>
         <r>
           <rPr>
@@ -1425,7 +1425,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D33" authorId="0" shapeId="0" xr:uid="{8EF2C23B-61AF-45D3-8657-64282A7B4EAA}">
+    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{E4DFC736-9D0F-4007-86A2-2EFB2D0E0A62}">
       <text>
         <r>
           <rPr>
@@ -1440,7 +1440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E33" authorId="0" shapeId="0" xr:uid="{63030813-7AFB-4C84-BAAA-315187903BD1}">
+    <comment ref="E23" authorId="0" shapeId="0" xr:uid="{2D359AEB-73C4-4525-A5E4-DC0D3E7D7D28}">
       <text>
         <r>
           <rPr>
@@ -1455,7 +1455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{B28C5B73-146E-4931-8054-9D9D77E8BE78}">
+    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{9034FECD-FBD4-4A02-AFFD-80D1A2C3D945}">
       <text>
         <r>
           <rPr>
@@ -1470,7 +1470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G33" authorId="0" shapeId="0" xr:uid="{BBFBD6B0-6835-4041-AF9C-FE4648FB66A7}">
+    <comment ref="G23" authorId="0" shapeId="0" xr:uid="{53F55730-8DF3-482C-AFFC-50A24453D837}">
       <text>
         <r>
           <rPr>
@@ -1485,7 +1485,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H33" authorId="0" shapeId="0" xr:uid="{641FBEB7-6B2F-49C1-B772-E258F225A11B}">
+    <comment ref="H23" authorId="0" shapeId="0" xr:uid="{8421E9CE-3722-48B9-AF04-8E2C202EEF46}">
       <text>
         <r>
           <rPr>
@@ -1500,7 +1500,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I33" authorId="0" shapeId="0" xr:uid="{6BAF4640-3A87-4D6D-AFE1-CA6D4354481A}">
+    <comment ref="I23" authorId="0" shapeId="0" xr:uid="{589D5876-8270-45F0-9AB5-839BF15D2BCF}">
       <text>
         <r>
           <rPr>
@@ -1515,7 +1515,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J33" authorId="0" shapeId="0" xr:uid="{CAA4BDEB-CC45-4391-9085-8EC7EDD99314}">
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{5E0179A7-138C-4BF5-8730-F635A8920960}">
       <text>
         <r>
           <rPr>
@@ -1530,7 +1530,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K33" authorId="0" shapeId="0" xr:uid="{42B0A39D-3FFF-4F67-A73D-AD680DE746F9}">
+    <comment ref="K23" authorId="0" shapeId="0" xr:uid="{5D625CCC-93E9-449B-A44F-37E8A3EC0360}">
       <text>
         <r>
           <rPr>
@@ -1545,7 +1545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L33" authorId="0" shapeId="0" xr:uid="{DAE51061-CC0D-41D5-82EF-F563114F292A}">
+    <comment ref="L23" authorId="0" shapeId="0" xr:uid="{F537D1B2-CFD7-445C-819D-9EEB3274FF99}">
       <text>
         <r>
           <rPr>
@@ -1560,7 +1560,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M33" authorId="0" shapeId="0" xr:uid="{CB42942D-2696-4EC1-B324-4500A39F41AD}">
+    <comment ref="M23" authorId="0" shapeId="0" xr:uid="{C00228D0-BCB0-4229-AB65-C27B659EB311}">
       <text>
         <r>
           <rPr>
@@ -1575,7 +1575,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N33" authorId="0" shapeId="0" xr:uid="{4BF9D25E-7018-47C4-9B16-224FDDA685BD}">
+    <comment ref="N23" authorId="0" shapeId="0" xr:uid="{3C77FB9B-07C2-4CA4-A803-79FCA1315FCF}">
       <text>
         <r>
           <rPr>
@@ -1590,7 +1590,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O33" authorId="0" shapeId="0" xr:uid="{97298C4C-4E20-48DB-A287-E620234F295E}">
+    <comment ref="O23" authorId="0" shapeId="0" xr:uid="{5CA4EA8F-16FA-4687-B6FD-816F9DBD1238}">
       <text>
         <r>
           <rPr>
@@ -1610,7 +1610,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
   <si>
     <t>project</t>
   </si>
@@ -1992,7 +1992,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2020,6 +2020,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="5"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Moneda 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -2398,6 +2399,203 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="15" width="13.6328125" customWidth="1"/>
+    <col min="16" max="17" width="20.08984375" customWidth="1"/>
+    <col min="18" max="19" width="21.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.5">
+      <c r="A1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.5">
+      <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.5">
+      <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.5">
+      <c r="A4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="5"/>
+    </row>
+    <row r="6" spans="1:15" s="7" customFormat="1" ht="31">
+      <c r="A6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.5">
+      <c r="A8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8">
+        <f>SUM($B7:$B7)</f>
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:O8" si="0">SUM($C7:$C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.5">
+      <c r="A9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
@@ -3254,209 +3452,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O9"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25141160-2363-4287-94F0-937880877F90}">
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="15" width="13.6328125" customWidth="1"/>
-    <col min="16" max="17" width="20.08984375" customWidth="1"/>
-    <col min="18" max="19" width="21.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="15.5">
-      <c r="A1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="4"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.5">
-      <c r="A2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.5">
-      <c r="A3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="5"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.5">
-      <c r="A4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="6" spans="1:15" s="7" customFormat="1" ht="31">
-      <c r="A6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.5">
-      <c r="A8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8">
-        <f>SUM($B7:$B7)</f>
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <f t="shared" ref="C8:O8" si="0">SUM($C7:$C7)</f>
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="15.5">
-      <c r="A9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE62EFC-2116-4319-8F77-90CB10608CAF}">
-  <dimension ref="A1:O33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
@@ -3548,7 +3549,7 @@
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" t="s">
+      <c r="A7" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="10">
@@ -3596,7 +3597,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.5" customHeight="1">
-      <c r="A8" t="s">
+      <c r="A8" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="10">
@@ -3604,7 +3605,7 @@
       </c>
       <c r="C8" s="10">
         <f>SUM(prj_monthly_justified_ensure)</f>
-        <v>11.833333333333334</v>
+        <v>12</v>
       </c>
       <c r="D8" s="10">
         <v>1</v>
@@ -3640,11 +3641,11 @@
         <v>1</v>
       </c>
       <c r="O8" s="10">
-        <v>0.83333333333333337</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.5" customHeight="1">
-      <c r="A9" t="s">
+      <c r="A9" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="10">
@@ -3652,7 +3653,7 @@
       </c>
       <c r="C9" s="10">
         <f>SUM(prj_monthly_justified_h2pcomplementario)</f>
-        <v>335.41666666666669</v>
+        <v>336</v>
       </c>
       <c r="D9" s="10">
         <v>28</v>
@@ -3688,11 +3689,11 @@
         <v>28</v>
       </c>
       <c r="O9" s="10">
-        <v>27.416666666666671</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" t="s">
+      <c r="A10" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="10">
@@ -3700,47 +3701,47 @@
       </c>
       <c r="C10" s="10">
         <f>SUM(prj_monthly_justified_pertevec_at10)</f>
-        <v>38.5</v>
+        <v>38.499999999999993</v>
       </c>
       <c r="D10" s="10">
-        <v>3.208333333333333</v>
+        <v>3.2</v>
       </c>
       <c r="E10" s="10">
-        <v>3.208333333333333</v>
+        <v>3.2</v>
       </c>
       <c r="F10" s="10">
-        <v>3.208333333333333</v>
+        <v>3.2</v>
       </c>
       <c r="G10" s="10">
-        <v>3.208333333333333</v>
+        <v>3.2</v>
       </c>
       <c r="H10" s="10">
-        <v>3.208333333333333</v>
+        <v>3.2</v>
       </c>
       <c r="I10" s="10">
-        <v>3.208333333333333</v>
+        <v>3.2</v>
       </c>
       <c r="J10" s="10">
-        <v>3.208333333333333</v>
+        <v>3.2</v>
       </c>
       <c r="K10" s="10">
-        <v>3.208333333333333</v>
+        <v>3.2</v>
       </c>
       <c r="L10" s="10">
-        <v>3.208333333333333</v>
+        <v>3.2</v>
       </c>
       <c r="M10" s="10">
-        <v>3.208333333333333</v>
+        <v>3.2</v>
       </c>
       <c r="N10" s="10">
-        <v>3.208333333333333</v>
+        <v>3.2</v>
       </c>
       <c r="O10" s="10">
-        <v>3.208333333333333</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" t="s">
+      <c r="A11" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="10">
@@ -3748,47 +3749,47 @@
       </c>
       <c r="C11" s="10">
         <f>SUM(prj_monthly_justified_pertevec_at15)</f>
-        <v>37.041666666666679</v>
+        <v>38</v>
       </c>
       <c r="D11" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="E11" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="F11" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="G11" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="H11" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="I11" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="J11" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="K11" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="L11" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="M11" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="N11" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="O11" s="10">
-        <v>2.208333333333333</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" t="s">
+      <c r="A12" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="10">
@@ -3796,47 +3797,47 @@
       </c>
       <c r="C12" s="10">
         <f>SUM(prj_monthly_justified_pertevec_at16)</f>
-        <v>38.000000000000007</v>
+        <v>38</v>
       </c>
       <c r="D12" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="E12" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="F12" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="G12" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="H12" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="I12" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="J12" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="K12" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="L12" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="M12" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="N12" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="O12" s="10">
-        <v>3.166666666666667</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" t="s">
+      <c r="A13" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="10">
@@ -3884,7 +3885,7 @@
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" t="s">
+      <c r="A14" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="10">
@@ -3892,47 +3893,47 @@
       </c>
       <c r="C14" s="10">
         <f>SUM(prj_monthly_justified_pertevec_at21)</f>
-        <v>38.000000000000007</v>
+        <v>38</v>
       </c>
       <c r="D14" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="E14" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="F14" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="G14" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="H14" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="I14" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="J14" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="K14" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="L14" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="M14" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="N14" s="10">
-        <v>3.166666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="O14" s="10">
-        <v>3.166666666666667</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" t="s">
+      <c r="A15" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="10">
@@ -3980,7 +3981,7 @@
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" t="s">
+      <c r="A16" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="10">
@@ -4028,7 +4029,7 @@
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" t="s">
+      <c r="A17" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="10">
@@ -4076,7 +4077,7 @@
       </c>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" t="s">
+      <c r="A18" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="10">
@@ -4084,7 +4085,7 @@
       </c>
       <c r="C18" s="10">
         <f>SUM(prj_monthly_justified_pilas)</f>
-        <v>28.708333333333332</v>
+        <v>30</v>
       </c>
       <c r="D18" s="10">
         <v>2.5</v>
@@ -4117,14 +4118,14 @@
         <v>2.5</v>
       </c>
       <c r="N18" s="10">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="O18" s="10">
-        <v>1.208333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" t="s">
+      <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="10">
@@ -4132,7 +4133,7 @@
       </c>
       <c r="C19" s="10">
         <f>SUM(prj_monthly_justified_porcino)</f>
-        <v>27.5</v>
+        <v>30</v>
       </c>
       <c r="D19" s="10">
         <v>2.5</v>
@@ -4165,649 +4166,169 @@
         <v>2.5</v>
       </c>
       <c r="N19" s="10">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="O19" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" t="s">
-        <v>31</v>
+      <c r="A20" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="B20" s="10">
-        <v>45</v>
+        <v>307.5</v>
       </c>
       <c r="C20" s="10">
-        <f>SUM(prj_monthly_justified_redol_wp1)</f>
-        <v>45</v>
-      </c>
-      <c r="D20" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="E20" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="F20" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="G20" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="H20" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="I20" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="J20" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="K20" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="L20" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="M20" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="N20" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="O20" s="10">
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="10">
-        <v>107</v>
-      </c>
-      <c r="C21" s="10">
-        <f>SUM(prj_monthly_justified_redol_wp2)</f>
-        <v>105.58333333333334</v>
-      </c>
-      <c r="D21" s="10">
-        <v>8.9166666666666661</v>
-      </c>
-      <c r="E21" s="10">
-        <v>8.9166666666666661</v>
-      </c>
-      <c r="F21" s="10">
-        <v>8.9166666666666661</v>
-      </c>
-      <c r="G21" s="10">
-        <v>8.9166666666666661</v>
-      </c>
-      <c r="H21" s="10">
-        <v>8.9166666666666661</v>
-      </c>
-      <c r="I21" s="10">
-        <v>8.9166666666666661</v>
-      </c>
-      <c r="J21" s="10">
-        <v>8.9166666666666661</v>
-      </c>
-      <c r="K21" s="10">
-        <v>8.9166666666666661</v>
-      </c>
-      <c r="L21" s="10">
-        <v>8.9166666666666661</v>
-      </c>
-      <c r="M21" s="10">
-        <v>8.9166666666666661</v>
-      </c>
-      <c r="N21" s="10">
-        <v>8.9166666666666661</v>
-      </c>
-      <c r="O21" s="10">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="10">
-        <v>5</v>
-      </c>
-      <c r="C22" s="10">
-        <f>SUM(prj_monthly_justified_redol_wp4)</f>
-        <v>4</v>
-      </c>
-      <c r="D22" s="10">
-        <v>0</v>
-      </c>
-      <c r="E22" s="10">
-        <v>0</v>
-      </c>
-      <c r="F22" s="10">
-        <v>0</v>
-      </c>
-      <c r="G22" s="10">
-        <v>0</v>
-      </c>
-      <c r="H22" s="10">
-        <v>0</v>
-      </c>
-      <c r="I22" s="10">
-        <v>0</v>
-      </c>
-      <c r="J22" s="10">
-        <v>0</v>
-      </c>
-      <c r="K22" s="10">
-        <v>1</v>
-      </c>
-      <c r="L22" s="10">
-        <v>1</v>
-      </c>
-      <c r="M22" s="10">
-        <v>1</v>
-      </c>
-      <c r="N22" s="10">
-        <v>1</v>
-      </c>
-      <c r="O22" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15">
-      <c r="A23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="10">
-        <v>18</v>
-      </c>
-      <c r="C23" s="10">
-        <f>SUM(prj_monthly_justified_redol_wp7)</f>
-        <v>18</v>
-      </c>
-      <c r="D23" s="10">
-        <v>0</v>
-      </c>
-      <c r="E23" s="10">
-        <v>0</v>
-      </c>
-      <c r="F23" s="10">
-        <v>0</v>
-      </c>
-      <c r="G23" s="10">
-        <v>0</v>
-      </c>
-      <c r="H23" s="10">
-        <v>0</v>
-      </c>
-      <c r="I23" s="10">
-        <v>0</v>
-      </c>
-      <c r="J23" s="10">
-        <v>0</v>
-      </c>
-      <c r="K23" s="10">
-        <v>0</v>
-      </c>
-      <c r="L23" s="10">
-        <v>4.5</v>
-      </c>
-      <c r="M23" s="10">
-        <v>4.5</v>
-      </c>
-      <c r="N23" s="10">
-        <v>4.5</v>
-      </c>
-      <c r="O23" s="10">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="A24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="10">
-        <v>45</v>
-      </c>
-      <c r="C24" s="10">
-        <f>SUM(prj_monthly_justified_redol_wp8)</f>
-        <v>45</v>
-      </c>
-      <c r="D24" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="E24" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="F24" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="G24" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="H24" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="I24" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="J24" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="K24" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="L24" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="M24" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="N24" s="10">
-        <v>3.75</v>
-      </c>
-      <c r="O24" s="10">
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="10">
-        <v>307.5</v>
-      </c>
-      <c r="C25" s="10">
         <f>SUM(prj_monthly_justified_reset)</f>
         <v>307.5</v>
       </c>
-      <c r="D25" s="10">
-        <v>25.625</v>
-      </c>
-      <c r="E25" s="10">
-        <v>25.625</v>
-      </c>
-      <c r="F25" s="10">
-        <v>25.625</v>
-      </c>
-      <c r="G25" s="10">
-        <v>25.625</v>
-      </c>
-      <c r="H25" s="10">
-        <v>25.625</v>
-      </c>
-      <c r="I25" s="10">
-        <v>25.625</v>
-      </c>
-      <c r="J25" s="10">
-        <v>25.625</v>
-      </c>
-      <c r="K25" s="10">
-        <v>25.625</v>
-      </c>
-      <c r="L25" s="10">
-        <v>25.625</v>
-      </c>
-      <c r="M25" s="10">
-        <v>25.625</v>
-      </c>
-      <c r="N25" s="10">
-        <v>25.625</v>
-      </c>
-      <c r="O25" s="10">
-        <v>25.625</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="A26" t="s">
+      <c r="D20" s="10">
         <v>26</v>
       </c>
-      <c r="B26" s="10">
-        <v>10</v>
-      </c>
-      <c r="C26" s="10">
-        <f>SUM(prj_monthly_justified_treasure_wp4)</f>
-        <v>9.1666666666666661</v>
-      </c>
-      <c r="D26" s="10">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E26" s="10">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="F26" s="10">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="G26" s="10">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="H26" s="10">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="I26" s="10">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="J26" s="10">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="K26" s="10">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="L26" s="10">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="M26" s="10">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="N26" s="10">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="O26" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="10">
-        <v>35</v>
-      </c>
-      <c r="C27" s="10">
-        <f>SUM(prj_monthly_justified_treasure_wp6)</f>
-        <v>32.083333333333343</v>
-      </c>
-      <c r="D27" s="10">
-        <v>2.916666666666667</v>
-      </c>
-      <c r="E27" s="10">
-        <v>2.916666666666667</v>
-      </c>
-      <c r="F27" s="10">
-        <v>2.916666666666667</v>
-      </c>
-      <c r="G27" s="10">
-        <v>2.916666666666667</v>
-      </c>
-      <c r="H27" s="10">
-        <v>2.916666666666667</v>
-      </c>
-      <c r="I27" s="10">
-        <v>2.916666666666667</v>
-      </c>
-      <c r="J27" s="10">
-        <v>2.916666666666667</v>
-      </c>
-      <c r="K27" s="10">
-        <v>2.916666666666667</v>
-      </c>
-      <c r="L27" s="10">
-        <v>2.916666666666667</v>
-      </c>
-      <c r="M27" s="10">
-        <v>2.916666666666667</v>
-      </c>
-      <c r="N27" s="10">
-        <v>2.916666666666667</v>
-      </c>
-      <c r="O27" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="10">
-        <v>75</v>
-      </c>
-      <c r="C28" s="10">
-        <f>SUM(prj_monthly_justified_treasure_wp7)</f>
-        <v>75</v>
-      </c>
-      <c r="D28" s="10">
-        <v>6.25</v>
-      </c>
-      <c r="E28" s="10">
-        <v>6.25</v>
-      </c>
-      <c r="F28" s="10">
-        <v>6.25</v>
-      </c>
-      <c r="G28" s="10">
-        <v>6.25</v>
-      </c>
-      <c r="H28" s="10">
-        <v>6.25</v>
-      </c>
-      <c r="I28" s="10">
-        <v>6.25</v>
-      </c>
-      <c r="J28" s="10">
-        <v>6.25</v>
-      </c>
-      <c r="K28" s="10">
-        <v>6.25</v>
-      </c>
-      <c r="L28" s="10">
-        <v>6.25</v>
-      </c>
-      <c r="M28" s="10">
-        <v>6.25</v>
-      </c>
-      <c r="N28" s="10">
-        <v>6.25</v>
-      </c>
-      <c r="O28" s="10">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="10">
-        <v>15</v>
-      </c>
-      <c r="C29" s="10">
-        <f>SUM(prj_monthly_justified_treasure_wp8)</f>
-        <v>13.75</v>
-      </c>
-      <c r="D29" s="10">
-        <v>1.25</v>
-      </c>
-      <c r="E29" s="10">
-        <v>1.25</v>
-      </c>
-      <c r="F29" s="10">
-        <v>1.25</v>
-      </c>
-      <c r="G29" s="10">
-        <v>1.25</v>
-      </c>
-      <c r="H29" s="10">
-        <v>1.25</v>
-      </c>
-      <c r="I29" s="10">
-        <v>1.25</v>
-      </c>
-      <c r="J29" s="10">
-        <v>1.25</v>
-      </c>
-      <c r="K29" s="10">
-        <v>1.25</v>
-      </c>
-      <c r="L29" s="10">
-        <v>1.25</v>
-      </c>
-      <c r="M29" s="10">
-        <v>1.25</v>
-      </c>
-      <c r="N29" s="10">
-        <v>1.25</v>
-      </c>
-      <c r="O29" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="10">
-        <v>5</v>
-      </c>
-      <c r="C30" s="10">
-        <f>SUM(prj_monthly_justified_treasure_wp9)</f>
-        <v>4.583333333333333</v>
-      </c>
-      <c r="D30" s="10">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="E30" s="10">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="F30" s="10">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="G30" s="10">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="H30" s="10">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="I30" s="10">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="J30" s="10">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="K30" s="10">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="L30" s="10">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="M30" s="10">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="N30" s="10">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="O30" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="15.5">
-      <c r="A32" s="6" t="s">
+      <c r="E20" s="10">
+        <v>26</v>
+      </c>
+      <c r="F20" s="10">
+        <v>26</v>
+      </c>
+      <c r="G20" s="10">
+        <v>26</v>
+      </c>
+      <c r="H20" s="10">
+        <v>26</v>
+      </c>
+      <c r="I20" s="10">
+        <v>26</v>
+      </c>
+      <c r="J20" s="10">
+        <v>26</v>
+      </c>
+      <c r="K20" s="10">
+        <v>25.5</v>
+      </c>
+      <c r="L20" s="10">
+        <v>25</v>
+      </c>
+      <c r="M20" s="10">
+        <v>25</v>
+      </c>
+      <c r="N20" s="10">
+        <v>25</v>
+      </c>
+      <c r="O20" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.5">
+      <c r="A22" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B22" s="10">
         <f>SUM(all_prj_projected)</f>
-        <v>1433</v>
-      </c>
-      <c r="C32" s="10">
+        <v>1073</v>
+      </c>
+      <c r="C22" s="10">
         <f>SUM(all_prj_justified)</f>
-        <v>1419.6666666666667</v>
-      </c>
-      <c r="D32" s="10">
+        <v>1073</v>
+      </c>
+      <c r="D22" s="10">
         <f>SUM(all_prj_monthly_justified_1)</f>
-        <v>110.5</v>
-      </c>
-      <c r="E32" s="10">
+        <v>83.033333333333331</v>
+      </c>
+      <c r="E22" s="10">
         <f>SUM(all_prj_monthly_justified_2)</f>
-        <v>110.5</v>
-      </c>
-      <c r="F32" s="10">
+        <v>83.033333333333331</v>
+      </c>
+      <c r="F22" s="10">
         <f>SUM(all_prj_monthly_justified_3)</f>
-        <v>110.5</v>
-      </c>
-      <c r="G32" s="10">
+        <v>83.033333333333331</v>
+      </c>
+      <c r="G22" s="10">
         <f>SUM(all_prj_monthly_justified_4)</f>
-        <v>110.5</v>
-      </c>
-      <c r="H32" s="10">
+        <v>83.033333333333331</v>
+      </c>
+      <c r="H22" s="10">
         <f>SUM(all_prj_monthly_justified_5)</f>
-        <v>110.5</v>
-      </c>
-      <c r="I32" s="10">
+        <v>83.033333333333331</v>
+      </c>
+      <c r="I22" s="10">
         <f>SUM(all_prj_monthly_justified_6)</f>
-        <v>110.5</v>
-      </c>
-      <c r="J32" s="10">
+        <v>83.033333333333331</v>
+      </c>
+      <c r="J22" s="10">
         <f>SUM(all_prj_monthly_justified_7)</f>
-        <v>113.66666666666667</v>
-      </c>
-      <c r="K32" s="10">
+        <v>86.2</v>
+      </c>
+      <c r="K22" s="10">
         <f>SUM(all_prj_monthly_justified_8)</f>
-        <v>114.66666666666667</v>
-      </c>
-      <c r="L32" s="10">
+        <v>85.7</v>
+      </c>
+      <c r="L22" s="10">
         <f>SUM(all_prj_monthly_justified_9)</f>
-        <v>119.16666666666667</v>
-      </c>
-      <c r="M32" s="10">
+        <v>85.2</v>
+      </c>
+      <c r="M22" s="10">
         <f>SUM(all_prj_monthly_justified_10)</f>
-        <v>144.16666666666666</v>
-      </c>
-      <c r="N32" s="10">
+        <v>110.2</v>
+      </c>
+      <c r="N22" s="10">
         <f>SUM(all_prj_monthly_justified_11)</f>
-        <v>139.16666666666666</v>
-      </c>
-      <c r="O32" s="10">
+        <v>109.2</v>
+      </c>
+      <c r="O22" s="10">
         <f>SUM(all_prj_monthly_justified_12)</f>
-        <v>125.83333333333333</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="15.5">
-      <c r="A33" s="6" t="s">
+        <v>98.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.5">
+      <c r="A23" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D23" s="10">
         <v>157.5</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E23" s="10">
         <v>150</v>
       </c>
-      <c r="F33" s="10">
+      <c r="F23" s="10">
         <v>172.5</v>
       </c>
-      <c r="G33" s="10">
+      <c r="G23" s="10">
         <v>135</v>
       </c>
-      <c r="H33" s="10">
+      <c r="H23" s="10">
         <v>165</v>
       </c>
-      <c r="I33" s="10">
+      <c r="I23" s="10">
         <v>165</v>
       </c>
-      <c r="J33" s="10">
+      <c r="J23" s="10">
         <v>157.5</v>
       </c>
-      <c r="K33" s="10">
+      <c r="K23" s="10">
         <v>165</v>
       </c>
-      <c r="L33" s="10">
+      <c r="L23" s="10">
         <v>157.5</v>
       </c>
-      <c r="M33" s="10">
+      <c r="M23" s="10">
         <v>157.5</v>
       </c>
-      <c r="N33" s="10">
+      <c r="N23" s="10">
         <v>157.5</v>
       </c>
-      <c r="O33" s="10">
+      <c r="O23" s="10">
         <v>127.5</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D7:O30">
+  <conditionalFormatting sqref="D7:O20">
     <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32:O32">
+  <conditionalFormatting sqref="D22:O22">
     <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
       <formula>INDIRECT("RC",FALSE) &gt; OFFSET(INDIRECT("RC",FALSE),1,0)</formula>
     </cfRule>
@@ -4818,7 +4339,7 @@
       <formula>INDIRECT("RC",FALSE) &lt; OFFSET(INDIRECT("RC",FALSE),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:C30">
+  <conditionalFormatting sqref="C7:C20">
     <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>INDIRECT("RC",FALSE) &gt; OFFSET(INDIRECT("RC",FALSE),0,-1)</formula>
     </cfRule>
@@ -4829,12 +4350,12 @@
       <formula>INDIRECT("RC",FALSE) &lt; OFFSET(INDIRECT("RC",FALSE),0,-1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32">
+  <conditionalFormatting sqref="B22">
     <cfRule type="expression" dxfId="1" priority="8" stopIfTrue="1">
-      <formula>$B$32 &gt; max_yearly_limit</formula>
+      <formula>$B$22 &gt; max_yearly_limit</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
-      <formula>$B$32 &lt;= max_yearly_limit</formula>
+      <formula>$B$22 &lt;= max_yearly_limit</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Added weekly report support
</commit_message>
<xml_diff>
--- a/resources/project-breakdown.xlsx
+++ b/resources/project-breakdown.xlsx
@@ -14,52 +14,52 @@
     <sheet name="John Smith - 2023" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_justified" vbProcedure="false">'John Smith - 2023'!$C$7:$C$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_justified_total" vbProcedure="false">'John Smith - 2023'!$C$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_monthly_justified_1" vbProcedure="false">'John Smith - 2023'!$D$7:$D$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_monthly_justified_10" vbProcedure="false">'John Smith - 2023'!$M$7:$M$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_monthly_justified_11" vbProcedure="false">'John Smith - 2023'!$N$7:$N$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_monthly_justified_12" vbProcedure="false">'John Smith - 2023'!$O$7:$O$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_monthly_justified_2" vbProcedure="false">'John Smith - 2023'!$E$7:$E$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_monthly_justified_3" vbProcedure="false">'John Smith - 2023'!$F$7:$F$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_monthly_justified_4" vbProcedure="false">'John Smith - 2023'!$G$7:$G$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_monthly_justified_5" vbProcedure="false">'John Smith - 2023'!$H$7:$H$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_monthly_justified_6" vbProcedure="false">'John Smith - 2023'!$I$7:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_monthly_justified_7" vbProcedure="false">'John Smith - 2023'!$J$7:$J$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_monthly_justified_8" vbProcedure="false">'John Smith - 2023'!$K$7:$K$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_monthly_justified_9" vbProcedure="false">'John Smith - 2023'!$L$7:$L$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_projected" vbProcedure="false">'John Smith - 2023'!$B$7:$B$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_projected_total" vbProcedure="false">'John Smith - 2023'!$B$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_justified" vbProcedure="false">'John Smith - 2023'!$C$7:$C$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_justified_total" vbProcedure="false">'John Smith - 2023'!$C$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_month_justified_1" vbProcedure="false">'John Smith - 2023'!$D$7:$D$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_month_justified_10" vbProcedure="false">'John Smith - 2023'!$M$7:$M$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_month_justified_11" vbProcedure="false">'John Smith - 2023'!$N$7:$N$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_month_justified_12" vbProcedure="false">'John Smith - 2023'!$O$7:$O$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_month_justified_2" vbProcedure="false">'John Smith - 2023'!$E$7:$E$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_month_justified_3" vbProcedure="false">'John Smith - 2023'!$F$7:$F$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_month_justified_4" vbProcedure="false">'John Smith - 2023'!$G$7:$G$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_month_justified_5" vbProcedure="false">'John Smith - 2023'!$H$7:$H$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_month_justified_6" vbProcedure="false">'John Smith - 2023'!$I$7:$I$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_month_justified_7" vbProcedure="false">'John Smith - 2023'!$J$7:$J$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_month_justified_8" vbProcedure="false">'John Smith - 2023'!$K$7:$K$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_month_justified_9" vbProcedure="false">'John Smith - 2023'!$L$7:$L$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_projected" vbProcedure="false">'John Smith - 2023'!$B$7:$B$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="all_prj_projected_total" vbProcedure="false">'John Smith - 2023'!$B$10</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="employee" vbProcedure="false">'John Smith - 2023'!$B$2</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="justification_year" vbProcedure="false">'John Smith - 2023'!$B$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="max_yearly_limit" vbProcedure="false">'John Smith - 2023'!$B$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_bioestilas" vbProcedure="false">'John Smith - 2023'!$D$7:$O$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_ensure" vbProcedure="false">'John Smith - 2023'!$D$8:$O$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_h2pcomplementario" vbProcedure="false">'John Smith - 2023'!$D$9:$O$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_pertevec_at10" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_pertevec_at15" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_pertevec_at16" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_pertevec_at2" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_pertevec_at21" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_pertevec_at3" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_pertevec_at4" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_pertevec_at9" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_pilas" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_porcino" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_redol_wp1" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_redol_wp2" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_redol_wp4" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_redol_wp7" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_redol_wp8" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_reset" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_treasure_wp4" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_treasure_wp6" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_treasure_wp7" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_treasure_wp8" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_monthly_justified_treasure_wp9" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_bioestilas" vbProcedure="false">'John Smith - 2023'!$D$7:$O$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_ensure" vbProcedure="false">'John Smith - 2023'!$D$8:$O$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_h2pcomplementario" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_pertevec_at10" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_pertevec_at15" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_pertevec_at16" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_pertevec_at2" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_pertevec_at21" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_pertevec_at3" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_pertevec_at4" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_pertevec_at9" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_pilas" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_porcino" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_redol_wp1" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_redol_wp2" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_redol_wp4" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_redol_wp7" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_redol_wp8" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_reset" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_treasure_wp4" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_treasure_wp6" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_treasure_wp7" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_treasure_wp8" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_month_justified_treasure_wp9" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="prj_total_justified_bioestilas" vbProcedure="false">'John Smith - 2023'!$C$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="prj_total_justified_ensure" vbProcedure="false">'John Smith - 2023'!$C$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_total_justified_h2pcomplementario" vbProcedure="false">'John Smith - 2023'!$C$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_total_justified_h2pcomplementario" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="prj_total_justified_pertevec_at10" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="prj_total_justified_pertevec_at15" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="prj_total_justified_pertevec_at16" vbProcedure="false">#REF!</definedName>
@@ -83,7 +83,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="prj_total_justified_treasure_wp9" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="prj_total_projected_bioestilas" vbProcedure="false">'John Smith - 2023'!$B$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="prj_total_projected_ensure" vbProcedure="false">'John Smith - 2023'!$B$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="prj_total_projected_h2pcomplementario" vbProcedure="false">'John Smith - 2023'!$B$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="prj_total_projected_h2pcomplementario" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="prj_total_projected_pertevec_at10" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="prj_total_projected_pertevec_at15" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="prj_total_projected_pertevec_at16" vbProcedure="false">#REF!</definedName>
@@ -988,7 +988,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="0">
+    <comment ref="A11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1078,7 +1078,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0">
+    <comment ref="B10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1108,7 +1108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0">
+    <comment ref="C10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1123,7 +1123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0">
+    <comment ref="D10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1139,7 +1139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0">
+    <comment ref="D11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1154,7 +1154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0">
+    <comment ref="E10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1170,7 +1170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0">
+    <comment ref="E11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1185,7 +1185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0">
+    <comment ref="F10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1201,7 +1201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0">
+    <comment ref="F11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1216,7 +1216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0">
+    <comment ref="G10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1232,7 +1232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="0">
+    <comment ref="G11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1247,7 +1247,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0">
+    <comment ref="H10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1263,7 +1263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H12" authorId="0">
+    <comment ref="H11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1278,7 +1278,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0">
+    <comment ref="I10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1294,7 +1294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0">
+    <comment ref="I11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1309,7 +1309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J11" authorId="0">
+    <comment ref="J10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1325,7 +1325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J12" authorId="0">
+    <comment ref="J11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1340,7 +1340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K11" authorId="0">
+    <comment ref="K10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1356,7 +1356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K12" authorId="0">
+    <comment ref="K11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1371,7 +1371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L11" authorId="0">
+    <comment ref="L10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1387,7 +1387,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L12" authorId="0">
+    <comment ref="L11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1402,7 +1402,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M11" authorId="0">
+    <comment ref="M10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1418,7 +1418,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M12" authorId="0">
+    <comment ref="M11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1433,7 +1433,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N11" authorId="0">
+    <comment ref="N10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1449,7 +1449,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N12" authorId="0">
+    <comment ref="N11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1464,7 +1464,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O11" authorId="0">
+    <comment ref="O10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1480,7 +1480,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O12" authorId="0">
+    <comment ref="O11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1500,7 +1500,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t xml:space="preserve">Each employee must have its own worksheet named after him/her.</t>
   </si>
@@ -1689,6 +1689,42 @@
   </si>
   <si>
     <t xml:space="preserve">John Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December</t>
   </si>
 </sst>
 </file>
@@ -1740,6 +1776,14 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
+      <color rgb="FFFEFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="&quot;Arial Narrow&quot;"/>
       <family val="0"/>
@@ -1748,14 +1792,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF375623"/>
-      <name val="&quot;Arial Narrow&quot;"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
       <name val="&quot;Arial Narrow&quot;"/>
       <family val="0"/>
       <charset val="1"/>
@@ -1792,6 +1828,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF8497B0"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFE7E6E6"/>
         <bgColor rgb="FFFCE4D6"/>
       </patternFill>
@@ -1806,12 +1848,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFCE4D6"/>
         <bgColor rgb="FFE7E6E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8497B0"/>
-        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
   </fills>
@@ -1863,7 +1899,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1903,12 +1939,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1917,28 +1956,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1953,7 +1988,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="25" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1966,7 +2009,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
@@ -1977,7 +2020,8 @@
     <cellStyle name="Normal 2" xfId="21"/>
     <cellStyle name="Normal 3" xfId="22"/>
     <cellStyle name="Normal 4" xfId="23"/>
-    <cellStyle name="StyleProjectName" xfId="24"/>
+    <cellStyle name="ReportHeader" xfId="24"/>
+    <cellStyle name="StyleProjectName" xfId="25"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -2057,7 +2101,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFCE4D6"/>
+      <rgbColor rgb="FFFEFFFF"/>
       <rgbColor rgb="FFE7E6E6"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -2073,7 +2117,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFCE4D6"/>
       <rgbColor rgb="FFFFE699"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -2111,17 +2155,17 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.63"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="101.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="89.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2145,10 +2189,10 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15.72"/>
@@ -2181,14 +2225,14 @@
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="6" s="7" customFormat="true" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="5" customFormat="true" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -2228,8 +2272,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="0" t="n">
@@ -2289,8 +2333,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="0" t="n">
@@ -2347,13 +2391,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:AZ29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.81"/>
@@ -2361,32 +2405,32 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="4" style="0" width="7.34"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+    <row r="1" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2394,10 +2438,10 @@
       <c r="A2" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="9" t="n">
+      <c r="B2" s="8" t="n">
         <v>45200</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="8" t="n">
         <v>45930</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -2423,10 +2467,10 @@
       <c r="A3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="9" t="n">
+      <c r="B3" s="8" t="n">
         <v>44896</v>
       </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="8" t="n">
         <v>45626</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -2452,10 +2496,10 @@
       <c r="A4" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="9" t="n">
+      <c r="B4" s="8" t="n">
         <v>44927</v>
       </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="8" t="n">
         <v>45930</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -2472,10 +2516,10 @@
       <c r="A5" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="9" t="n">
+      <c r="B5" s="8" t="n">
         <v>44743</v>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="8" t="n">
         <v>44926</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -2501,10 +2545,10 @@
       <c r="A6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="9" t="n">
+      <c r="B6" s="8" t="n">
         <v>44743</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="8" t="n">
         <v>45838</v>
       </c>
       <c r="D6" s="0" t="n">
@@ -2530,10 +2574,10 @@
       <c r="A7" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="9" t="n">
+      <c r="B7" s="8" t="n">
         <v>44743</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="8" t="n">
         <v>45838</v>
       </c>
       <c r="D7" s="0" t="n">
@@ -2559,10 +2603,10 @@
       <c r="A8" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="9" t="n">
+      <c r="B8" s="8" t="n">
         <v>44743</v>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="8" t="n">
         <v>45838</v>
       </c>
       <c r="D8" s="0" t="n">
@@ -2588,10 +2632,10 @@
       <c r="A9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="9" t="n">
+      <c r="B9" s="8" t="n">
         <v>44743</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="8" t="n">
         <v>45473</v>
       </c>
       <c r="D9" s="0" t="n">
@@ -2617,10 +2661,10 @@
       <c r="A10" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="9" t="n">
+      <c r="B10" s="8" t="n">
         <v>44743</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="8" t="n">
         <v>45838</v>
       </c>
       <c r="D10" s="0" t="n">
@@ -2646,10 +2690,10 @@
       <c r="A11" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="9" t="n">
+      <c r="B11" s="8" t="n">
         <v>44743</v>
       </c>
-      <c r="C11" s="9" t="n">
+      <c r="C11" s="8" t="n">
         <v>45838</v>
       </c>
       <c r="D11" s="0" t="n">
@@ -2675,10 +2719,10 @@
       <c r="A12" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="9" t="n">
+      <c r="B12" s="8" t="n">
         <v>45108</v>
       </c>
-      <c r="C12" s="9" t="n">
+      <c r="C12" s="8" t="n">
         <v>45838</v>
       </c>
       <c r="D12" s="0" t="n">
@@ -2704,10 +2748,10 @@
       <c r="A13" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="9" t="n">
+      <c r="B13" s="8" t="n">
         <v>44743</v>
       </c>
-      <c r="C13" s="9" t="n">
+      <c r="C13" s="8" t="n">
         <v>45838</v>
       </c>
       <c r="D13" s="0" t="n">
@@ -2733,10 +2777,10 @@
       <c r="A14" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="9" t="n">
+      <c r="B14" s="8" t="n">
         <v>44835</v>
       </c>
-      <c r="C14" s="9" t="n">
+      <c r="C14" s="8" t="n">
         <v>45565</v>
       </c>
       <c r="D14" s="0" t="n">
@@ -2762,10 +2806,10 @@
       <c r="A15" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="9" t="n">
+      <c r="B15" s="8" t="n">
         <v>44835</v>
       </c>
-      <c r="C15" s="9" t="n">
+      <c r="C15" s="8" t="n">
         <v>45565</v>
       </c>
       <c r="D15" s="0" t="n">
@@ -2791,10 +2835,10 @@
       <c r="A16" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="9" t="n">
+      <c r="B16" s="8" t="n">
         <v>44896</v>
       </c>
-      <c r="C16" s="9" t="n">
+      <c r="C16" s="8" t="n">
         <v>46356</v>
       </c>
       <c r="D16" s="0" t="n">
@@ -2820,10 +2864,10 @@
       <c r="A17" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="9" t="n">
+      <c r="B17" s="8" t="n">
         <v>44896</v>
       </c>
-      <c r="C17" s="9" t="n">
+      <c r="C17" s="8" t="n">
         <v>45351</v>
       </c>
       <c r="D17" s="0" t="n">
@@ -2849,10 +2893,10 @@
       <c r="A18" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="9" t="n">
+      <c r="B18" s="8" t="n">
         <v>45139</v>
       </c>
-      <c r="C18" s="9" t="n">
+      <c r="C18" s="8" t="n">
         <v>45869</v>
       </c>
       <c r="D18" s="0" t="n">
@@ -2878,10 +2922,10 @@
       <c r="A19" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="9" t="n">
+      <c r="B19" s="8" t="n">
         <v>45170</v>
       </c>
-      <c r="C19" s="9" t="n">
+      <c r="C19" s="8" t="n">
         <v>46356</v>
       </c>
       <c r="D19" s="0" t="n">
@@ -2907,10 +2951,10 @@
       <c r="A20" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="9" t="n">
+      <c r="B20" s="8" t="n">
         <v>44896</v>
       </c>
-      <c r="C20" s="9" t="n">
+      <c r="C20" s="8" t="n">
         <v>46356</v>
       </c>
       <c r="D20" s="0" t="n">
@@ -2936,10 +2980,10 @@
       <c r="A21" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="9" t="n">
+      <c r="B21" s="8" t="n">
         <v>44440</v>
       </c>
-      <c r="C21" s="9" t="n">
+      <c r="C21" s="8" t="n">
         <v>45535</v>
       </c>
       <c r="D21" s="0" t="n">
@@ -2965,10 +3009,10 @@
       <c r="A22" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="9" t="n">
+      <c r="B22" s="8" t="n">
         <v>44348</v>
       </c>
-      <c r="C22" s="9" t="n">
+      <c r="C22" s="8" t="n">
         <v>44895</v>
       </c>
       <c r="D22" s="0" t="n">
@@ -2994,10 +3038,10 @@
       <c r="A23" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="9" t="n">
+      <c r="B23" s="8" t="n">
         <v>44348</v>
       </c>
-      <c r="C23" s="9" t="n">
+      <c r="C23" s="8" t="n">
         <v>45260</v>
       </c>
       <c r="D23" s="0" t="n">
@@ -3023,10 +3067,10 @@
       <c r="A24" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="9" t="n">
+      <c r="B24" s="8" t="n">
         <v>44348</v>
       </c>
-      <c r="C24" s="9" t="n">
+      <c r="C24" s="8" t="n">
         <v>44895</v>
       </c>
       <c r="D24" s="0" t="n">
@@ -3052,10 +3096,10 @@
       <c r="A25" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="9" t="n">
+      <c r="B25" s="8" t="n">
         <v>44348</v>
       </c>
-      <c r="C25" s="9" t="n">
+      <c r="C25" s="8" t="n">
         <v>45443</v>
       </c>
       <c r="D25" s="0" t="n">
@@ -3076,15 +3120,16 @@
       <c r="I25" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="AZ25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="9" t="n">
+      <c r="B26" s="8" t="n">
         <v>44866</v>
       </c>
-      <c r="C26" s="9" t="n">
+      <c r="C26" s="8" t="n">
         <v>45443</v>
       </c>
       <c r="D26" s="0" t="n">
@@ -3110,10 +3155,10 @@
       <c r="A27" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="9" t="n">
+      <c r="B27" s="8" t="n">
         <v>44348</v>
       </c>
-      <c r="C27" s="9" t="n">
+      <c r="C27" s="8" t="n">
         <v>45443</v>
       </c>
       <c r="D27" s="0" t="n">
@@ -3139,10 +3184,10 @@
       <c r="A28" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="9" t="n">
+      <c r="B28" s="8" t="n">
         <v>44348</v>
       </c>
-      <c r="C28" s="9" t="n">
+      <c r="C28" s="8" t="n">
         <v>45443</v>
       </c>
       <c r="D28" s="0" t="n">
@@ -3168,10 +3213,10 @@
       <c r="A29" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="9" t="n">
+      <c r="B29" s="8" t="n">
         <v>44348</v>
       </c>
-      <c r="C29" s="9" t="n">
+      <c r="C29" s="8" t="n">
         <v>45443</v>
       </c>
       <c r="D29" s="0" t="n">
@@ -3212,24 +3257,16 @@
   <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="24.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="8.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="9.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="5.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="6.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="10" width="5.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="5.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="10" width="8.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="10" width="6.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="10" width="8.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="10" width="7.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="10" width="20.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="10" width="21.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="19.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="8.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="6.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="4" style="9" width="5.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="16" style="9" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3264,299 +3301,252 @@
         <v>1433</v>
       </c>
     </row>
-    <row r="6" s="7" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+    <row r="6" s="11" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="D6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="13" t="n">
+        <v>65</v>
+      </c>
+      <c r="C7" s="13" t="n">
+        <f aca="false">SUM(prj_month_justified_bioestilas)</f>
+        <v>65</v>
+      </c>
+      <c r="D7" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="13" t="n">
+        <v>20</v>
+      </c>
+      <c r="N7" s="13" t="n">
+        <v>25</v>
+      </c>
+      <c r="O7" s="13" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="13" t="n">
         <v>12</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="12" t="n">
-        <v>65</v>
-      </c>
-      <c r="C7" s="12" t="n">
-        <f aca="false">SUM(prj_monthly_justified_bioestilas)</f>
-        <v>65</v>
-      </c>
-      <c r="D7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="12" t="n">
-        <v>25</v>
-      </c>
-      <c r="N7" s="12" t="n">
-        <v>20</v>
-      </c>
-      <c r="O7" s="12" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="12" t="n">
+      <c r="C8" s="13" t="n">
+        <f aca="false">SUM(prj_month_justified_ensure)</f>
         <v>12</v>
       </c>
-      <c r="C8" s="12" t="n">
-        <f aca="false">SUM(prj_monthly_justified_ensure)</f>
-        <v>12</v>
-      </c>
-      <c r="D8" s="12" t="n">
+      <c r="D8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="12" t="n">
+      <c r="E8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="12" t="n">
+      <c r="F8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="12" t="n">
+      <c r="G8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="H8" s="12" t="n">
+      <c r="H8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="12" t="n">
+      <c r="I8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="J8" s="12" t="n">
+      <c r="J8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="K8" s="12" t="n">
+      <c r="K8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="L8" s="12" t="n">
+      <c r="L8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="M8" s="12" t="n">
+      <c r="M8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="N8" s="12" t="n">
+      <c r="N8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O8" s="12" t="n">
+      <c r="O8" s="13" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="12" t="n">
-        <v>336</v>
-      </c>
-      <c r="C9" s="12" t="n">
-        <f aca="false">SUM(prj_monthly_justified_h2pcomplementario)</f>
-        <v>336</v>
-      </c>
-      <c r="D9" s="12" t="n">
-        <v>28</v>
-      </c>
-      <c r="E9" s="12" t="n">
-        <v>27</v>
-      </c>
-      <c r="F9" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="G9" s="12" t="n">
-        <v>25</v>
-      </c>
-      <c r="H9" s="12" t="n">
-        <v>30</v>
-      </c>
-      <c r="I9" s="12" t="n">
-        <v>30</v>
-      </c>
-      <c r="J9" s="12" t="n">
-        <v>28</v>
-      </c>
-      <c r="K9" s="12" t="n">
-        <v>30</v>
-      </c>
-      <c r="L9" s="12" t="n">
-        <v>28</v>
-      </c>
-      <c r="M9" s="12" t="n">
-        <v>28</v>
-      </c>
-      <c r="N9" s="12" t="n">
-        <v>28</v>
-      </c>
-      <c r="O9" s="12" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="13" t="n">
+      <c r="B10" s="14" t="n">
         <f aca="false">SUM(all_prj_projected)</f>
-        <v>413</v>
-      </c>
-      <c r="C11" s="13" t="n">
+        <v>77</v>
+      </c>
+      <c r="C10" s="14" t="n">
         <f aca="false">SUM(all_prj_justified)</f>
-        <v>413</v>
-      </c>
-      <c r="D11" s="13" t="n">
-        <f aca="false">SUM(all_prj_monthly_justified_1)</f>
-        <v>29</v>
-      </c>
-      <c r="E11" s="13" t="n">
-        <f aca="false">SUM(all_prj_monthly_justified_2)</f>
-        <v>28</v>
-      </c>
-      <c r="F11" s="13" t="n">
-        <f aca="false">SUM(all_prj_monthly_justified_3)</f>
-        <v>32</v>
-      </c>
-      <c r="G11" s="13" t="n">
-        <f aca="false">SUM(all_prj_monthly_justified_4)</f>
+        <v>77</v>
+      </c>
+      <c r="D10" s="14" t="n">
+        <f aca="false">SUM(all_prj_month_justified_1)</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="14" t="n">
+        <f aca="false">SUM(all_prj_month_justified_2)</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="14" t="n">
+        <f aca="false">SUM(all_prj_month_justified_3)</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="14" t="n">
+        <f aca="false">SUM(all_prj_month_justified_4)</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="14" t="n">
+        <f aca="false">SUM(all_prj_month_justified_5)</f>
+        <v>1</v>
+      </c>
+      <c r="I10" s="14" t="n">
+        <f aca="false">SUM(all_prj_month_justified_6)</f>
+        <v>1</v>
+      </c>
+      <c r="J10" s="14" t="n">
+        <f aca="false">SUM(all_prj_month_justified_7)</f>
+        <v>1</v>
+      </c>
+      <c r="K10" s="14" t="n">
+        <f aca="false">SUM(all_prj_month_justified_8)</f>
+        <v>1</v>
+      </c>
+      <c r="L10" s="14" t="n">
+        <f aca="false">SUM(all_prj_month_justified_9)</f>
+        <v>1</v>
+      </c>
+      <c r="M10" s="14" t="n">
+        <f aca="false">SUM(all_prj_month_justified_10)</f>
+        <v>21</v>
+      </c>
+      <c r="N10" s="14" t="n">
+        <f aca="false">SUM(all_prj_month_justified_11)</f>
         <v>26</v>
       </c>
-      <c r="H11" s="13" t="n">
-        <f aca="false">SUM(all_prj_monthly_justified_5)</f>
-        <v>31</v>
-      </c>
-      <c r="I11" s="13" t="n">
-        <f aca="false">SUM(all_prj_monthly_justified_6)</f>
-        <v>31</v>
-      </c>
-      <c r="J11" s="13" t="n">
-        <f aca="false">SUM(all_prj_monthly_justified_7)</f>
-        <v>29</v>
-      </c>
-      <c r="K11" s="13" t="n">
-        <f aca="false">SUM(all_prj_monthly_justified_8)</f>
-        <v>31</v>
-      </c>
-      <c r="L11" s="13" t="n">
-        <f aca="false">SUM(all_prj_monthly_justified_9)</f>
-        <v>29</v>
-      </c>
-      <c r="M11" s="13" t="n">
-        <f aca="false">SUM(all_prj_monthly_justified_10)</f>
-        <v>54</v>
-      </c>
-      <c r="N11" s="13" t="n">
-        <f aca="false">SUM(all_prj_monthly_justified_11)</f>
-        <v>49</v>
-      </c>
-      <c r="O11" s="13" t="n">
-        <f aca="false">SUM(all_prj_monthly_justified_12)</f>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="O10" s="14" t="n">
+        <f aca="false">SUM(all_prj_month_justified_12)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="13" t="n">
+      <c r="D11" s="14" t="n">
         <v>157.5</v>
       </c>
-      <c r="E12" s="13" t="n">
+      <c r="E11" s="14" t="n">
         <v>150</v>
       </c>
-      <c r="F12" s="13" t="n">
+      <c r="F11" s="14" t="n">
         <v>172.5</v>
       </c>
-      <c r="G12" s="13" t="n">
+      <c r="G11" s="14" t="n">
         <v>135</v>
       </c>
-      <c r="H12" s="13" t="n">
+      <c r="H11" s="14" t="n">
         <v>165</v>
       </c>
-      <c r="I12" s="13" t="n">
+      <c r="I11" s="14" t="n">
         <v>165</v>
       </c>
-      <c r="J12" s="13" t="n">
+      <c r="J11" s="14" t="n">
         <v>157.5</v>
       </c>
-      <c r="K12" s="13" t="n">
+      <c r="K11" s="14" t="n">
         <v>165</v>
       </c>
-      <c r="L12" s="13" t="n">
+      <c r="L11" s="14" t="n">
         <v>157.5</v>
       </c>
-      <c r="M12" s="13" t="n">
+      <c r="M11" s="14" t="n">
         <v>157.5</v>
       </c>
-      <c r="N12" s="13" t="n">
+      <c r="N11" s="14" t="n">
         <v>157.5</v>
       </c>
-      <c r="O12" s="13" t="n">
+      <c r="O11" s="14" t="n">
         <v>127.5</v>
       </c>
     </row>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3579,12 +3569,12 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="D7:O9">
+  <conditionalFormatting sqref="D7:O8">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11:O11">
+  <conditionalFormatting sqref="D10:O10">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>INDIRECT("RC",0) &gt; OFFSET(INDIRECT("RC",0),1,0)</formula>
     </cfRule>
@@ -3595,7 +3585,7 @@
       <formula>INDIRECT("RC",0) &lt; OFFSET(INDIRECT("RC",0),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:C9">
+  <conditionalFormatting sqref="C7:C8">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>INDIRECT("RC",0) &gt; OFFSET(INDIRECT("RC",0),0,-1)</formula>
     </cfRule>
@@ -3606,12 +3596,12 @@
       <formula>INDIRECT("RC",0) &lt; OFFSET(INDIRECT("RC",0),0,-1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
+  <conditionalFormatting sqref="B10">
     <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>$B$11 &gt; #NAME?</formula>
+      <formula>$B$10 &gt; #name?</formula>
     </cfRule>
     <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>$B$11 &lt;= #NAME?</formula>
+      <formula>$B$10 &lt;= #name?</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>